<commit_message>
docs: Update Product Backlog
</commit_message>
<xml_diff>
--- a/backlog-do-produto.xlsx
+++ b/backlog-do-produto.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
   <si>
     <t>RANK</t>
   </si>
@@ -343,7 +343,7 @@
         <color theme="1"/>
         <sz val="13.0"/>
       </rPr>
-      <t xml:space="preserve">botão de navegação para fazer o quiz </t>
+      <t>quiz após cada capítulo</t>
     </r>
     <r>
       <rPr>
@@ -351,7 +351,7 @@
         <color theme="1"/>
         <sz val="13.0"/>
       </rPr>
-      <t>após cada capítulo, para verificar se absorvi o conteúdo capítulo</t>
+      <t>, para verificar se absorvi o conteúdo capítulo</t>
     </r>
   </si>
   <si>
@@ -370,7 +370,7 @@
         <color theme="1"/>
         <sz val="13.0"/>
       </rPr>
-      <t>perguntas simples do conteúdo</t>
+      <t>perguntas do conteúdo</t>
     </r>
     <r>
       <rPr>
@@ -397,7 +397,7 @@
         <color theme="1"/>
         <sz val="13.0"/>
       </rPr>
-      <t xml:space="preserve">botão para refazer o quiz </t>
+      <t>botão de navegação para fazer o exame final</t>
     </r>
     <r>
       <rPr>
@@ -405,7 +405,7 @@
         <color theme="1"/>
         <sz val="13.0"/>
       </rPr>
-      <t>caso não me sinta satisfeito com o resultado</t>
+      <t>, para verificar se absorvi todo o conteúdo</t>
     </r>
   </si>
   <si>
@@ -415,7 +415,7 @@
         <color theme="1"/>
         <sz val="13.0"/>
       </rPr>
-      <t xml:space="preserve">Como usuário estudante de Scrum, quero um </t>
+      <t xml:space="preserve">Como o cliente que requisita a aplicação, quero um </t>
     </r>
     <r>
       <rPr>
@@ -424,7 +424,7 @@
         <color theme="1"/>
         <sz val="13.0"/>
       </rPr>
-      <t>botão de navegação para fazer o exame final de cada tema</t>
+      <t xml:space="preserve">sistema de login, </t>
     </r>
     <r>
       <rPr>
@@ -432,7 +432,7 @@
         <color theme="1"/>
         <sz val="13.0"/>
       </rPr>
-      <t>, para verificar se absorvi o conteúdo do tema</t>
+      <t xml:space="preserve">para salvar os dados dos usuários, tanto nos quizz quanto exames </t>
     </r>
   </si>
   <si>
@@ -451,7 +451,7 @@
         <color theme="1"/>
         <sz val="13.0"/>
       </rPr>
-      <t>perguntas medias/complexas sobre o todo o tema abordado</t>
+      <t>mais conteúdo sobre metodologias ágeis</t>
     </r>
     <r>
       <rPr>
@@ -459,7 +459,7 @@
         <color theme="1"/>
         <sz val="13.0"/>
       </rPr>
-      <t>, para que eu possa ser avaliado sobre o meu aprendizado por completo</t>
+      <t>, para que eu possa aprender tais habilidades</t>
     </r>
   </si>
   <si>
@@ -469,7 +469,7 @@
         <color theme="1"/>
         <sz val="13.0"/>
       </rPr>
-      <t xml:space="preserve">Como usuário estudante de Scrum, quero um </t>
+      <t xml:space="preserve">Como usuário estudante de Scrum, quero </t>
     </r>
     <r>
       <rPr>
@@ -478,15 +478,7 @@
         <color theme="1"/>
         <sz val="13.0"/>
       </rPr>
-      <t xml:space="preserve">botão para refazer o exame final </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="13.0"/>
-      </rPr>
-      <t>de cada tema caso não me sinta satisfeito com o resultado</t>
+      <t>quiz e exame funcionando</t>
     </r>
   </si>
   <si>
@@ -513,7 +505,78 @@
         <color theme="1"/>
         <sz val="13.0"/>
       </rPr>
-      <t>no teste final</t>
+      <t>em cada quizz que fizer</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="13.0"/>
+      </rPr>
+      <t xml:space="preserve">Como o cliente que requisita a aplicação, quero uma </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="13.0"/>
+      </rPr>
+      <t>tela de resultados</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="13.0"/>
+      </rPr>
+      <t xml:space="preserve"> para ver a proficiencia de cada usuário estudante, capaz de </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="13.0"/>
+      </rPr>
+      <t>ver todas as vezes que esse usuário realizar</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="13.0"/>
+      </rPr>
+      <t xml:space="preserve"> o curso</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="13.0"/>
+      </rPr>
+      <t xml:space="preserve">Como o cliente que requisita a aplicação, quero que o meu usuário estudante tenha seu </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="13.0"/>
+      </rPr>
+      <t>nome e a sua avaliação</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="13.0"/>
+      </rPr>
+      <t xml:space="preserve"> sobre o site na tela de resultados</t>
     </r>
   </si>
   <si>
@@ -535,7 +598,7 @@
         <color theme="1"/>
         <sz val="13.0"/>
       </rPr>
-      <t>mostre as alternativas certas e erradas após o envio do exame final</t>
+      <t xml:space="preserve">mostre a correcão das alternativas erradas </t>
     </r>
     <r>
       <rPr>
@@ -543,7 +606,7 @@
         <color theme="1"/>
         <sz val="13.0"/>
       </rPr>
-      <t>, para analisar onde errei</t>
+      <t>após o envio do exame final, para analisar onde errei</t>
     </r>
   </si>
   <si>
@@ -578,7 +641,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -596,8 +659,17 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -610,6 +682,18 @@
         <bgColor rgb="FFC9DAF8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor rgb="FFD9EAD3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4CCCC"/>
+        <bgColor rgb="FFF4CCCC"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -617,36 +701,57 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -871,12 +976,20 @@
     <col customWidth="1" min="6" max="6" width="9.25"/>
   </cols>
   <sheetData>
-    <row r="1" ht="5.25" customHeight="1">
+    <row r="1" ht="30.0" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -899,19 +1012,19 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>0</v>
+    <row r="2" ht="30.0" customHeight="1">
+      <c r="A2" s="1"/>
+      <c r="B2" s="3">
+        <v>1.0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>2</v>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>3</v>
+      <c r="E2" s="3">
+        <v>1.0</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -935,17 +1048,17 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" ht="38.25" customHeight="1">
-      <c r="A3" s="2"/>
-      <c r="B3" s="4">
-        <v>1.0</v>
+      <c r="A3" s="1"/>
+      <c r="B3" s="3">
+        <v>2.0</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>5</v>
+      <c r="D3" s="4" t="s">
+        <v>6</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>1.0</v>
       </c>
       <c r="G3" s="1"/>
@@ -970,17 +1083,17 @@
       <c r="Z3" s="1"/>
     </row>
     <row r="4">
-      <c r="A4" s="2"/>
-      <c r="B4" s="4">
-        <v>2.0</v>
+      <c r="A4" s="5"/>
+      <c r="B4" s="3">
+        <v>3.0</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>1.0</v>
       </c>
       <c r="G4" s="1"/>
@@ -1005,17 +1118,17 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="2"/>
-      <c r="B5" s="4">
-        <v>3.0</v>
+      <c r="A5" s="5"/>
+      <c r="B5" s="3">
+        <v>4.0</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>1.0</v>
       </c>
       <c r="G5" s="1"/>
@@ -1040,17 +1153,17 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6">
-      <c r="A6" s="2"/>
-      <c r="B6" s="4">
-        <v>4.0</v>
+      <c r="A6" s="5"/>
+      <c r="B6" s="3">
+        <v>5.0</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>1.0</v>
       </c>
       <c r="G6" s="1"/>
@@ -1075,17 +1188,17 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7">
-      <c r="A7" s="2"/>
-      <c r="B7" s="4">
-        <v>5.0</v>
+      <c r="A7" s="5"/>
+      <c r="B7" s="3">
+        <v>6.0</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>1.0</v>
       </c>
       <c r="G7" s="1"/>
@@ -1110,18 +1223,18 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8">
-      <c r="A8" s="2"/>
-      <c r="B8" s="4">
-        <v>6.0</v>
+      <c r="A8" s="5"/>
+      <c r="B8" s="3">
+        <v>7.0</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
-      <c r="E8" s="4">
-        <v>1.0</v>
+      <c r="E8" s="3">
+        <v>2.0</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1145,17 +1258,17 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9">
-      <c r="A9" s="2"/>
-      <c r="B9" s="4">
-        <v>7.0</v>
+      <c r="A9" s="5"/>
+      <c r="B9" s="3">
+        <v>8.0</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>2.0</v>
       </c>
       <c r="G9" s="1"/>
@@ -1180,17 +1293,17 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10">
-      <c r="A10" s="2"/>
-      <c r="B10" s="4">
-        <v>8.0</v>
+      <c r="A10" s="5"/>
+      <c r="B10" s="3">
+        <v>9.0</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>2.0</v>
       </c>
       <c r="G10" s="1"/>
@@ -1215,17 +1328,17 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11">
-      <c r="A11" s="2"/>
-      <c r="B11" s="4">
-        <v>9.0</v>
+      <c r="A11" s="5"/>
+      <c r="B11" s="3">
+        <v>10.0</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>4</v>
+      <c r="C11" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>2.0</v>
       </c>
       <c r="G11" s="1"/>
@@ -1250,17 +1363,17 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12">
-      <c r="A12" s="2"/>
-      <c r="B12" s="4">
-        <v>10.0</v>
+      <c r="A12" s="5"/>
+      <c r="B12" s="3">
+        <v>11.0</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>2.0</v>
       </c>
       <c r="G12" s="1"/>
@@ -1285,17 +1398,17 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13">
-      <c r="A13" s="2"/>
-      <c r="B13" s="4">
-        <v>11.0</v>
+      <c r="A13" s="5"/>
+      <c r="B13" s="3">
+        <v>12.0</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>2.0</v>
       </c>
       <c r="G13" s="1"/>
@@ -1320,18 +1433,18 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14">
-      <c r="A14" s="2"/>
-      <c r="B14" s="4">
-        <v>12.0</v>
+      <c r="A14" s="5"/>
+      <c r="B14" s="3">
+        <v>13.0</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
-      <c r="E14" s="4">
-        <v>3.0</v>
+      <c r="E14" s="3">
+        <v>2.0</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1354,19 +1467,19 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15">
-      <c r="A15" s="2"/>
-      <c r="B15" s="4">
-        <v>13.0</v>
+    <row r="15" ht="34.5" customHeight="1">
+      <c r="A15" s="5"/>
+      <c r="B15" s="3">
+        <v>14.0</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
-      <c r="E15" s="4">
-        <v>3.0</v>
+      <c r="E15" s="3">
+        <v>2.0</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -1390,17 +1503,17 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16">
-      <c r="A16" s="2"/>
-      <c r="B16" s="4">
-        <v>14.0</v>
+      <c r="A16" s="5"/>
+      <c r="B16" s="3">
+        <v>15.0</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>14</v>
+      <c r="C16" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>3.0</v>
       </c>
       <c r="G16" s="1"/>
@@ -1425,17 +1538,17 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17">
-      <c r="A17" s="2"/>
-      <c r="B17" s="4">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6">
         <v>15.0</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>20</v>
+      <c r="D17" s="7" t="s">
+        <v>21</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="8">
         <v>3.0</v>
       </c>
       <c r="G17" s="1"/>
@@ -1459,18 +1572,18 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18">
-      <c r="A18" s="2"/>
-      <c r="B18" s="4">
+    <row r="18" ht="26.25" customHeight="1">
+      <c r="A18" s="5"/>
+      <c r="B18" s="3">
         <v>16.0</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="3">
         <v>3.0</v>
       </c>
       <c r="G18" s="1"/>
@@ -1495,17 +1608,17 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19">
-      <c r="A19" s="2"/>
-      <c r="B19" s="4">
+      <c r="A19" s="5"/>
+      <c r="B19" s="3">
         <v>17.0</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="3">
         <v>3.0</v>
       </c>
       <c r="G19" s="1"/>
@@ -1530,18 +1643,18 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20">
-      <c r="A20" s="2"/>
-      <c r="B20" s="4">
+      <c r="A20" s="5"/>
+      <c r="B20" s="9">
         <v>18.0</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>14</v>
+      <c r="C20" s="10" t="s">
+        <v>4</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>23</v>
+      <c r="D20" s="11" t="s">
+        <v>24</v>
       </c>
-      <c r="E20" s="4">
-        <v>3.0</v>
+      <c r="E20" s="9">
+        <v>4.0</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -1564,79 +1677,92 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21">
-      <c r="A21" s="2"/>
-      <c r="B21" s="4">
+    <row r="21" ht="42.75" customHeight="1">
+      <c r="A21" s="12"/>
+      <c r="B21" s="9">
         <v>19.0</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>24</v>
+      <c r="C21" s="13" t="s">
+        <v>4</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="9">
         <v>4.0</v>
       </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-      <c r="T21" s="1"/>
-      <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
-      <c r="W21" s="1"/>
-      <c r="X21" s="1"/>
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="1"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="2"/>
-      <c r="B22" s="4">
+      <c r="F21" s="14"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="12"/>
+      <c r="T21" s="12"/>
+      <c r="U21" s="12"/>
+      <c r="V21" s="12"/>
+      <c r="W21" s="12"/>
+      <c r="X21" s="12"/>
+      <c r="Y21" s="12"/>
+      <c r="Z21" s="12"/>
+    </row>
+    <row r="22" ht="45.75" customHeight="1">
+      <c r="A22" s="12"/>
+      <c r="B22" s="6">
         <v>20.0</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="4" t="s">
+      <c r="C22" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E22" s="4">
+      <c r="D22" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="6">
         <v>4.0</v>
       </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
-      <c r="T22" s="1"/>
-      <c r="U22" s="1"/>
-      <c r="V22" s="1"/>
-      <c r="W22" s="1"/>
-      <c r="X22" s="1"/>
-      <c r="Y22" s="1"/>
-      <c r="Z22" s="1"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="12"/>
+      <c r="T22" s="12"/>
+      <c r="U22" s="12"/>
+      <c r="V22" s="12"/>
+      <c r="W22" s="12"/>
+      <c r="X22" s="12"/>
+      <c r="Y22" s="12"/>
+      <c r="Z22" s="12"/>
     </row>
     <row r="23">
-      <c r="A23" s="2"/>
-      <c r="B23" s="4"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="6">
+        <v>21.0</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="6">
+        <v>4.0</v>
+      </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -1659,11 +1785,11 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24">
-      <c r="A24" s="6"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
+      <c r="A24" s="5"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -1686,11 +1812,11 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="15"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -1713,12 +1839,11 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="9"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>

</xml_diff>

<commit_message>
Fix Backlog do Produto
</commit_message>
<xml_diff>
--- a/backlog-do-produto.xlsx
+++ b/backlog-do-produto.xlsx
@@ -669,30 +669,12 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC9DAF8"/>
-        <bgColor rgb="FFC9DAF8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD9EAD3"/>
-        <bgColor rgb="FFD9EAD3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4CCCC"/>
-        <bgColor rgb="FFF4CCCC"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -701,57 +683,42 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1014,16 +981,16 @@
     </row>
     <row r="2" ht="30.0" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>1.0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>1.0</v>
       </c>
       <c r="G2" s="1"/>
@@ -1049,16 +1016,16 @@
     </row>
     <row r="3" ht="38.25" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>2.0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>1.0</v>
       </c>
       <c r="G3" s="1"/>
@@ -1083,17 +1050,17 @@
       <c r="Z3" s="1"/>
     </row>
     <row r="4">
-      <c r="A4" s="5"/>
-      <c r="B4" s="3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="2">
         <v>3.0</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>1.0</v>
       </c>
       <c r="G4" s="1"/>
@@ -1118,17 +1085,17 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="5"/>
-      <c r="B5" s="3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="2">
         <v>4.0</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>1.0</v>
       </c>
       <c r="G5" s="1"/>
@@ -1153,17 +1120,17 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6">
-      <c r="A6" s="5"/>
-      <c r="B6" s="3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="2">
         <v>5.0</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>1.0</v>
       </c>
       <c r="G6" s="1"/>
@@ -1188,17 +1155,17 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7">
-      <c r="A7" s="5"/>
-      <c r="B7" s="3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="2">
         <v>6.0</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>1.0</v>
       </c>
       <c r="G7" s="1"/>
@@ -1223,17 +1190,17 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8">
-      <c r="A8" s="5"/>
-      <c r="B8" s="3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="2">
         <v>7.0</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>2.0</v>
       </c>
       <c r="G8" s="1"/>
@@ -1258,17 +1225,17 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9">
-      <c r="A9" s="5"/>
-      <c r="B9" s="3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="2">
         <v>8.0</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>2.0</v>
       </c>
       <c r="G9" s="1"/>
@@ -1293,17 +1260,17 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10">
-      <c r="A10" s="5"/>
-      <c r="B10" s="3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="2">
         <v>9.0</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>2.0</v>
       </c>
       <c r="G10" s="1"/>
@@ -1328,17 +1295,17 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11">
-      <c r="A11" s="5"/>
-      <c r="B11" s="3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="2">
         <v>10.0</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>2.0</v>
       </c>
       <c r="G11" s="1"/>
@@ -1363,17 +1330,17 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12">
-      <c r="A12" s="5"/>
-      <c r="B12" s="3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="2">
         <v>11.0</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>2.0</v>
       </c>
       <c r="G12" s="1"/>
@@ -1398,17 +1365,17 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13">
-      <c r="A13" s="5"/>
-      <c r="B13" s="3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="2">
         <v>12.0</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>2.0</v>
       </c>
       <c r="G13" s="1"/>
@@ -1433,17 +1400,17 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14">
-      <c r="A14" s="5"/>
-      <c r="B14" s="3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="2">
         <v>13.0</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <v>2.0</v>
       </c>
       <c r="G14" s="1"/>
@@ -1468,17 +1435,17 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" ht="34.5" customHeight="1">
-      <c r="A15" s="5"/>
-      <c r="B15" s="3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="2">
         <v>14.0</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <v>2.0</v>
       </c>
       <c r="G15" s="1"/>
@@ -1503,17 +1470,17 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16">
-      <c r="A16" s="5"/>
-      <c r="B16" s="3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="2">
         <v>15.0</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <v>3.0</v>
       </c>
       <c r="G16" s="1"/>
@@ -1538,17 +1505,17 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6">
+      <c r="A17" s="4"/>
+      <c r="B17" s="2">
         <v>15.0</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="5">
         <v>3.0</v>
       </c>
       <c r="G17" s="1"/>
@@ -1573,17 +1540,17 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" ht="26.25" customHeight="1">
-      <c r="A18" s="5"/>
-      <c r="B18" s="3">
+      <c r="A18" s="4"/>
+      <c r="B18" s="2">
         <v>16.0</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="2">
         <v>3.0</v>
       </c>
       <c r="G18" s="1"/>
@@ -1608,17 +1575,17 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19">
-      <c r="A19" s="5"/>
-      <c r="B19" s="3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="2">
         <v>17.0</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <v>3.0</v>
       </c>
       <c r="G19" s="1"/>
@@ -1643,17 +1610,17 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20">
-      <c r="A20" s="5"/>
-      <c r="B20" s="9">
+      <c r="A20" s="4"/>
+      <c r="B20" s="6">
         <v>18.0</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="6">
         <v>4.0</v>
       </c>
       <c r="G20" s="1"/>
@@ -1678,89 +1645,89 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" ht="42.75" customHeight="1">
-      <c r="A21" s="12"/>
-      <c r="B21" s="9">
+      <c r="A21" s="9"/>
+      <c r="B21" s="6">
         <v>19.0</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="6">
         <v>4.0</v>
       </c>
-      <c r="F21" s="14"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="12"/>
-      <c r="Q21" s="12"/>
-      <c r="R21" s="12"/>
-      <c r="S21" s="12"/>
-      <c r="T21" s="12"/>
-      <c r="U21" s="12"/>
-      <c r="V21" s="12"/>
-      <c r="W21" s="12"/>
-      <c r="X21" s="12"/>
-      <c r="Y21" s="12"/>
-      <c r="Z21" s="12"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="9"/>
     </row>
     <row r="22" ht="45.75" customHeight="1">
-      <c r="A22" s="12"/>
-      <c r="B22" s="6">
+      <c r="A22" s="9"/>
+      <c r="B22" s="2">
         <v>20.0</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="2">
         <v>4.0</v>
       </c>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="12"/>
-      <c r="P22" s="12"/>
-      <c r="Q22" s="12"/>
-      <c r="R22" s="12"/>
-      <c r="S22" s="12"/>
-      <c r="T22" s="12"/>
-      <c r="U22" s="12"/>
-      <c r="V22" s="12"/>
-      <c r="W22" s="12"/>
-      <c r="X22" s="12"/>
-      <c r="Y22" s="12"/>
-      <c r="Z22" s="12"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="9"/>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="9"/>
+      <c r="Z22" s="9"/>
     </row>
     <row r="23">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6">
+      <c r="A23" s="4"/>
+      <c r="B23" s="2">
         <v>21.0</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="2">
         <v>4.0</v>
       </c>
       <c r="G23" s="1"/>
@@ -1785,11 +1752,11 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24">
-      <c r="A24" s="5"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -1812,11 +1779,11 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="15"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="2"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -1839,11 +1806,11 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26">
-      <c r="A26" s="5"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>

</xml_diff>